<commit_message>
New 3D Files & AVG Profile
</commit_message>
<xml_diff>
--- a/Firmware/SD-Files/SD-Files/profiles/PowderList.xlsx
+++ b/Firmware/SD-Files/SD-Files/profiles/PowderList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Powder</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Pc (kg/m³)</t>
   </si>
   <si>
+    <t xml:space="preserve">AVG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Blue Dot</t>
   </si>
   <si>
@@ -88,10 +91,10 @@
     <t xml:space="preserve">N320</t>
   </si>
   <si>
+    <t xml:space="preserve">N32c</t>
+  </si>
+  <si>
     <t xml:space="preserve">N340</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N32c</t>
   </si>
   <si>
     <t xml:space="preserve">RS 14</t>
@@ -104,18 +107,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="168" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,6 +138,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -180,29 +183,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -214,6 +213,15 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -222,411 +230,432 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="1" t="n">
+        <f aca="false">ROUND(AVERAGE(B3:B23),3)</f>
+        <v>9.126</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <f aca="false">ROUND(AVERAGE(C3:C23),3)</f>
+        <v>0.591</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">ROUND(AVERAGE(D3:D23),0)</f>
+        <v>806</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">ROUND(AVERAGE(E3:E23),0)</f>
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="n">
         <v>7.50139562646</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <f aca="false">B2/15.4323583529</f>
+      <c r="C3" s="3" t="n">
+        <f aca="false">B3/15.4323583529</f>
         <v>0.48608226007468</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>775</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>1590</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="n">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="n">
         <v>7.55159317143</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <f aca="false">B3/15.4323583529</f>
+      <c r="C4" s="3" t="n">
+        <f aca="false">B4/15.4323583529</f>
         <v>0.489335006273421</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>610</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>980</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="n">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="n">
         <v>11.3309440056</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <f aca="false">B4/15.4323583529</f>
+      <c r="C5" s="3" t="n">
+        <f aca="false">B5/15.4323583529</f>
         <v>0.734232820835885</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>950</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>1590</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="n">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="n">
         <v>7.78605402022</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <f aca="false">B5/15.4323583529</f>
+      <c r="C6" s="3" t="n">
+        <f aca="false">B6/15.4323583529</f>
         <v>0.504527813712729</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>986</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>1570</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="n">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="n">
         <v>9.52815792765</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <f aca="false">B6/15.4323583529</f>
+      <c r="C7" s="3" t="n">
+        <f aca="false">B7/15.4323583529</f>
         <v>0.617414248021237</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>860</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>1670</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="n">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="n">
         <v>11.5816929268</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <f aca="false">B7/15.4323583529</f>
+      <c r="C8" s="3" t="n">
+        <f aca="false">B8/15.4323583529</f>
         <v>0.750481077613365</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>986</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>1540</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3" t="n">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="n">
         <v>11.7935070365</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <f aca="false">B8/15.4323583529</f>
+      <c r="C9" s="3" t="n">
+        <f aca="false">B9/15.4323583529</f>
         <v>0.764206401044582</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>970</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>1580</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="n">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="n">
         <v>9.90719301668</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <f aca="false">B9/15.4323583529</f>
+      <c r="C10" s="3" t="n">
+        <f aca="false">B10/15.4323583529</f>
         <v>0.641975308642199</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>970</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>1680</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="n">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="n">
         <v>10.8313492939</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <f aca="false">B10/15.4323583529</f>
+      <c r="C11" s="3" t="n">
+        <f aca="false">B11/15.4323583529</f>
         <v>0.701859628075874</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>960</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>1620</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="n">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="n">
         <v>9.61440855852</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <f aca="false">B11/15.4323583529</f>
+      <c r="C12" s="3" t="n">
+        <f aca="false">B12/15.4323583529</f>
         <v>0.62300319488844</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>840</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>1510</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="n">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="n">
         <v>8.32834837311</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <f aca="false">B12/15.4323583529</f>
+      <c r="C13" s="3" t="n">
+        <f aca="false">B13/15.4323583529</f>
         <v>0.53966789667925</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>870</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>1550</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="n">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4" t="n">
         <v>8.8271128198</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <f aca="false">B13/15.4323583529</f>
+      <c r="C14" s="3" t="n">
+        <f aca="false">B14/15.4323583529</f>
         <v>0.571987289171602</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>920</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>1680</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="n">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4" t="n">
         <v>12.499729507</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <f aca="false">B14/15.4323583529</f>
+      <c r="C15" s="3" t="n">
+        <f aca="false">B15/15.4323583529</f>
         <v>0.809968847350612</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>979</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>1560</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3" t="n">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="n">
         <v>13.8306084051</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <f aca="false">B15/15.4323583529</f>
+      <c r="C16" s="3" t="n">
+        <f aca="false">B16/15.4323583529</f>
         <v>0.896208349289725</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>890</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>1580</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="3" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="4" t="n">
         <v>11.4169201852</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <f aca="false">B16/15.4323583529</f>
+      <c r="C17" s="3" t="n">
+        <f aca="false">B17/15.4323583529</f>
         <v>0.739803983559944</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>920</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>1590</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3" t="n">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="4" t="n">
         <v>5.69855113552</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <f aca="false">B17/15.4323583529</f>
+      <c r="C18" s="3" t="n">
+        <f aca="false">B18/15.4323583529</f>
         <v>0.36925990216195</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>560</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>1540</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="3" t="n">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="4" t="n">
         <v>7.74264977397</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <f aca="false">B18/15.4323583529</f>
+      <c r="C19" s="3" t="n">
+        <f aca="false">B19/15.4323583529</f>
         <v>0.501715265866349</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>550</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>1220</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="3" t="n">
-        <v>7.65727704533</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <f aca="false">B19/15.4323583529</f>
-        <v>0.496183206106737</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>620</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>1690</v>
-      </c>
-    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="4" t="n">
         <v>5.71387951674</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="3" t="n">
         <f aca="false">B20/15.4323583529</f>
         <v>0.370253164557073</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>420</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>1490</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="4" t="n">
+        <v>7.65727704533</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <f aca="false">B21/15.4323583529</f>
+        <v>0.496183206106737</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>620</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="4" t="n">
         <v>2.6080975405</v>
       </c>
-      <c r="C21" s="2" t="n">
-        <f aca="false">B21/15.4323583529</f>
+      <c r="C22" s="3" t="n">
+        <f aca="false">B22/15.4323583529</f>
         <v>0.169001877798535</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>316</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>1600</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3" t="n">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4" t="n">
         <v>9.90447573938</v>
       </c>
-      <c r="C22" s="2" t="n">
-        <f aca="false">B22/15.4323583529</f>
+      <c r="C23" s="3" t="n">
+        <f aca="false">B23/15.4323583529</f>
         <v>0.641799232034991</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>976</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>1610</v>
       </c>
     </row>

</xml_diff>